<commit_message>
adicionado para remover colunas com "0"
</commit_message>
<xml_diff>
--- a/data/func.xlsx
+++ b/data/func.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esocial9\Desktop\AutoJoin\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniel Costa\OneDrive\Desktop\GitHubProjetos\AutoJoin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F758D26C-E06F-4EB5-9AEB-9453C2367B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB10D21B-43FB-4A85-B21C-9EF853C9836D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,16 +722,16 @@
     <tableColumn id="4" xr3:uid="{55593206-F501-4B1B-8F38-7638AC2FC474}" name="CPF" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{27DBF3A5-0EB9-450A-8ACE-20B74444F268}" name="RUA" dataDxfId="11"/>
     <tableColumn id="6" xr3:uid="{326BE118-DC53-47BB-B58C-1BAF0B7992D9}" name="NOME_PAI" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{6E748758-AC23-4E11-AC0D-5A1F971BA1EB}" name="NOME_MAE" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{616C724E-E6F6-43F3-9BE0-78183815043D}" name="NUMERO" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{4BD4F5A2-A67B-4F7B-9A62-B5DA8C07848F}" name="COMPLEMENTO" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{34C9BE10-85EF-4988-BA25-AC6971ECE0BF}" name="BAIRRO" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{52BAFDDA-2367-4EEE-A85D-94BA646774C8}" name="MUNICIPIO" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{3F628F3C-2F12-4DFA-96AF-1073A0E668FA}" name="UF" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{E52607E0-7154-4962-9796-49D483D56DC0}" name="CEP" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{C2FE7E5F-CD5A-4938-A169-D790E424F526}" name="DDD" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{708DCFDF-EADB-44D8-A4B3-3A02490A35A5}" name="CELULAR" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{F40175EC-1BE3-4C7D-AE9C-CFE5C85CAF71}" name="FONE" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{6E748758-AC23-4E11-AC0D-5A1F971BA1EB}" name="NOME_MAE" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{616C724E-E6F6-43F3-9BE0-78183815043D}" name="NUMERO" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{4BD4F5A2-A67B-4F7B-9A62-B5DA8C07848F}" name="COMPLEMENTO" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{34C9BE10-85EF-4988-BA25-AC6971ECE0BF}" name="BAIRRO" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{52BAFDDA-2367-4EEE-A85D-94BA646774C8}" name="MUNICIPIO" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{3F628F3C-2F12-4DFA-96AF-1073A0E668FA}" name="UF" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{E52607E0-7154-4962-9796-49D483D56DC0}" name="CEP" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{C2FE7E5F-CD5A-4938-A169-D790E424F526}" name="DDD" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{708DCFDF-EADB-44D8-A4B3-3A02490A35A5}" name="CELULAR" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{F40175EC-1BE3-4C7D-AE9C-CFE5C85CAF71}" name="FONE" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,6 +1137,9 @@
       <c r="O2" t="s">
         <v>29</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1154,6 +1157,21 @@
       <c r="E3" t="s">
         <v>34</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1171,6 +1189,21 @@
       <c r="E4" t="s">
         <v>42</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1215,6 +1248,9 @@
       <c r="O5" t="s">
         <v>29</v>
       </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1229,11 +1265,20 @@
       <c r="D6" t="s">
         <v>54</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
       <c r="N6" t="s">
         <v>28</v>
       </c>
       <c r="O6" t="s">
         <v>29</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1255,6 +1300,9 @@
       <c r="G7" t="s">
         <v>36</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="J7" t="s">
         <v>59</v>
       </c>
@@ -1272,6 +1320,9 @@
       </c>
       <c r="O7" t="s">
         <v>61</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1317,6 +1368,9 @@
       <c r="O8" t="s">
         <v>70</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1361,6 +1415,9 @@
       <c r="O9" t="s">
         <v>29</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1378,6 +1435,9 @@
       <c r="E10" t="s">
         <v>82</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="J10" t="s">
         <v>55</v>
       </c>
@@ -1395,6 +1455,9 @@
       </c>
       <c r="O10" t="s">
         <v>29</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1413,6 +1476,9 @@
       <c r="F11" t="s">
         <v>35</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="J11" t="s">
         <v>88</v>
       </c>
@@ -1430,6 +1496,9 @@
       </c>
       <c r="O11" t="s">
         <v>90</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1448,17 +1517,26 @@
       <c r="G12" t="s">
         <v>36</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
       <c r="K12" t="s">
         <v>50</v>
       </c>
       <c r="L12" t="s">
         <v>26</v>
       </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="N12" t="s">
         <v>28</v>
       </c>
       <c r="O12" t="s">
         <v>94</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1483,6 +1561,21 @@
       <c r="G13" t="s">
         <v>100</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1506,6 +1599,21 @@
       <c r="G14" t="s">
         <v>106</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1526,11 +1634,20 @@
       <c r="G15" t="s">
         <v>36</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="N15" t="s">
         <v>28</v>
       </c>
       <c r="O15" t="s">
         <v>110</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>